<commit_message>
[0413] Fix Template Cow Import
</commit_message>
<xml_diff>
--- a/src/main/resources/static/document/cow_import_template.xlsx
+++ b/src/main/resources/static/document/cow_import_template.xlsx
@@ -1337,7 +1337,7 @@
   <dimension ref="A1:R101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1424,8 +1424,8 @@
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
       <c r="K2" s="12" t="str">
-        <f ca="1">IF(Q2&lt;&gt;"",UPPER(LEFT(Q2,1))&amp;"-0006"&amp;"-"&amp;TEXT(COUNTIF($G$2:P2,Q2),"0000"),"")</f>
-        <v>N-0006-0000</v>
+        <f>IF(Q2&lt;&gt;"",UPPER(LEFT(Q2,1))&amp;"-0006"&amp;"-"&amp;TEXT(COUNTIF($Q$2:Q3,Q2),"0000"),"")</f>
+        <v>N-0006-0001</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>9</v>

</xml_diff>